<commit_message>
Server ICO Change & client path change
</commit_message>
<xml_diff>
--- a/Table/xlsx/Item.xlsx
+++ b/Table/xlsx/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shlif\OneDrive\Documents\GitHub\MyDetectiveServer\Table\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D1139B-93EF-4BC1-8724-05816EC927FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F4F9B9-CE0C-4AD7-9E9D-1E84CF05769D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -597,10 +597,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">가죽 벨트입니다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>대상은 45초 이후 죽게됩니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1065,6 +1061,10 @@
   </si>
   <si>
     <t>Job</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">가죽 벨트입니다. 상대를 목졸라 죽일 수 있습니다. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1645,9 +1645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showFormulas="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1684,7 +1684,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>10</v>
@@ -1699,16 +1699,16 @@
         <v>20</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -1731,7 +1731,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>9</v>
@@ -1746,10 +1746,10 @@
         <v>19</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>74</v>
@@ -1778,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H3" s="10" t="b">
         <v>1</v>
@@ -1793,16 +1793,16 @@
         <v>1</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" s="11" t="b">
         <v>1</v>
@@ -1840,16 +1840,16 @@
         <v>1</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1872,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H5" s="11" t="b">
         <v>1</v>
@@ -1887,16 +1887,16 @@
         <v>1</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1919,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" s="11" t="b">
         <v>1</v>
@@ -1934,16 +1934,16 @@
         <v>1</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1966,7 +1966,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H7" s="11" t="b">
         <v>1</v>
@@ -1981,16 +1981,16 @@
         <v>1</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2013,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H8" s="11" t="b">
         <v>1</v>
@@ -2028,16 +2028,16 @@
         <v>1</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2060,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" s="11" t="b">
         <v>1</v>
@@ -2075,16 +2075,16 @@
         <v>1</v>
       </c>
       <c r="L9" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="M9" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="M9" s="23" t="s">
-        <v>186</v>
-      </c>
       <c r="N9" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H10" s="11" t="b">
         <v>1</v>
@@ -2122,16 +2122,16 @@
         <v>1</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H11" s="11" t="b">
         <v>1</v>
@@ -2169,16 +2169,16 @@
         <v>0</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2201,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H12" s="11" t="b">
         <v>1</v>
@@ -2216,16 +2216,16 @@
         <v>0</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H13" s="11" t="b">
         <v>1</v>
@@ -2263,16 +2263,16 @@
         <v>1</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2295,7 +2295,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="11" t="b">
         <v>1</v>
@@ -2310,16 +2310,16 @@
         <v>0</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H15" s="11" t="b">
         <v>1</v>
@@ -2357,16 +2357,16 @@
         <v>0</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M15" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2389,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H16" s="11" t="b">
         <v>1</v>
@@ -2404,16 +2404,16 @@
         <v>0</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M16" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2436,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H17" s="11" t="b">
         <v>1</v>
@@ -2451,16 +2451,16 @@
         <v>0</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M17" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2483,7 +2483,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H18" s="11" t="b">
         <v>1</v>
@@ -2498,16 +2498,16 @@
         <v>0</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M18" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2530,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H19" s="11" t="b">
         <v>1</v>
@@ -2545,16 +2545,16 @@
         <v>1</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M19" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2568,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E20" s="11">
         <v>1</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H20" s="11" t="b">
         <v>1</v>
@@ -2586,22 +2586,22 @@
         <v>1</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K20" s="18" t="b">
         <v>1</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H21" s="11" t="b">
         <v>1</v>
@@ -2639,16 +2639,16 @@
         <v>1</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M21" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H22" s="11" t="b">
         <v>1</v>
@@ -2686,16 +2686,16 @@
         <v>1</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M22" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H23" s="11" t="b">
         <v>1</v>
@@ -2733,16 +2733,16 @@
         <v>1</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M23" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2765,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H24" s="11" t="b">
         <v>1</v>
@@ -2780,16 +2780,16 @@
         <v>1</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M24" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H25" s="11" t="b">
         <v>1</v>
@@ -2827,16 +2827,16 @@
         <v>1</v>
       </c>
       <c r="L25" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="M25" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="M25" s="23" t="s">
-        <v>186</v>
-      </c>
       <c r="N25" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H26" s="11" t="b">
         <v>1</v>
@@ -2874,16 +2874,16 @@
         <v>1</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M26" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H27" s="11" t="b">
         <v>1</v>
@@ -2921,16 +2921,16 @@
         <v>1</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M27" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2953,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H28" s="11" t="b">
         <v>1</v>
@@ -2968,16 +2968,16 @@
         <v>0</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M28" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3000,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H29" s="11" t="b">
         <v>1</v>
@@ -3015,16 +3015,16 @@
         <v>0</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H30" s="11" t="b">
         <v>1</v>
@@ -3062,16 +3062,16 @@
         <v>0</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M30" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -3094,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H31" s="11" t="b">
         <v>1</v>
@@ -3109,16 +3109,16 @@
         <v>1</v>
       </c>
       <c r="L31" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="M31" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="M31" s="23" t="s">
-        <v>186</v>
-      </c>
       <c r="N31" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -3126,7 +3126,7 @@
         <v>130</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="11">
         <v>1</v>
@@ -3141,7 +3141,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H32" s="11" t="b">
         <v>1</v>
@@ -3156,16 +3156,16 @@
         <v>0</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M32" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3186,7 +3186,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3221,7 +3221,7 @@
         <v>101</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>43</v>
@@ -3232,7 +3232,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>44</v>
@@ -3243,7 +3243,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>45</v>
@@ -3254,7 +3254,7 @@
         <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>46</v>
@@ -3265,7 +3265,7 @@
         <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>47</v>
@@ -3276,7 +3276,7 @@
         <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
@@ -3287,7 +3287,7 @@
         <v>107</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>48</v>
@@ -3298,7 +3298,7 @@
         <v>108</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>51</v>
@@ -3309,7 +3309,7 @@
         <v>109</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>52</v>
@@ -3320,7 +3320,7 @@
         <v>110</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>53</v>
@@ -3331,7 +3331,7 @@
         <v>111</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>54</v>
@@ -3342,7 +3342,7 @@
         <v>112</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>49</v>
@@ -3353,7 +3353,7 @@
         <v>113</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>50</v>
@@ -3364,7 +3364,7 @@
         <v>114</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>55</v>
@@ -3375,7 +3375,7 @@
         <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>56</v>
@@ -3386,7 +3386,7 @@
         <v>116</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>57</v>
@@ -3397,7 +3397,7 @@
         <v>117</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>58</v>
@@ -3408,7 +3408,7 @@
         <v>118</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>59</v>
@@ -3419,7 +3419,7 @@
         <v>119</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>60</v>
@@ -3430,7 +3430,7 @@
         <v>120</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>61</v>
@@ -3441,7 +3441,7 @@
         <v>121</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>62</v>
@@ -3452,7 +3452,7 @@
         <v>122</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>63</v>
@@ -3463,7 +3463,7 @@
         <v>123</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>64</v>
@@ -3474,7 +3474,7 @@
         <v>124</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>65</v>
@@ -3485,7 +3485,7 @@
         <v>125</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>66</v>
@@ -3496,7 +3496,7 @@
         <v>126</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>67</v>
@@ -3507,7 +3507,7 @@
         <v>127</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>71</v>
@@ -3518,7 +3518,7 @@
         <v>128</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>72</v>
@@ -3529,7 +3529,7 @@
         <v>129</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>73</v>
@@ -3540,10 +3540,10 @@
         <v>130</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3557,8 +3557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCC9497-2FBF-43DB-BB52-14FC0A9E0A69}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3773,7 +3773,7 @@
         <v>58</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -3784,7 +3784,7 @@
         <v>59</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -3795,7 +3795,7 @@
         <v>60</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3806,7 +3806,7 @@
         <v>61</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -3817,7 +3817,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -3828,7 +3828,7 @@
         <v>63</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -3839,7 +3839,7 @@
         <v>64</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -3850,7 +3850,7 @@
         <v>65</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -3861,7 +3861,7 @@
         <v>66</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -3872,7 +3872,7 @@
         <v>67</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -3883,7 +3883,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -3894,7 +3894,7 @@
         <v>72</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.3">
@@ -3905,7 +3905,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -3913,10 +3913,10 @@
         <v>130</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>